<commit_message>
ajuste layout novos começos
</commit_message>
<xml_diff>
--- a/Consolidado_Bridge_2025.xlsx
+++ b/Consolidado_Bridge_2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08d87aadaabdc2cb/Documentos/nwb/bridge/dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08d87aadaabdc2cb/Desktop/BRIDGE/consolidado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="8_{C607EACA-C650-4A5E-95C7-07DDA7668303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6240D3A7-ED12-4002-8728-A9293F1F3CD6}"/>
+  <xr:revisionPtr revIDLastSave="234" documentId="8_{C607EACA-C650-4A5E-95C7-07DDA7668303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48C26579-51CD-49A7-B372-D15CDFD40AAD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EEFB68E0-0739-433A-A945-0FEA615287DD}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="2025 Consolidado" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025 Consolidado'!$A$1:$P$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'2025 Consolidado'!$A$1:$O$135</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1935" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="552">
   <si>
     <t>Quando</t>
   </si>
@@ -1525,7 +1525,195 @@
     <t>Conseguiu fazer contato?</t>
   </si>
   <si>
-    <t>Formula</t>
+    <t>Rodrigo Almeida</t>
+  </si>
+  <si>
+    <t>21 99604-1664</t>
+  </si>
+  <si>
+    <t>Entrei em contato e o dono do número informou que o número estava errado.Na verdade era uma mulher chamada Camila. Ela informou que o número estava errado e eu a convidei assim mesmo para conhecer nossa igreja.
+Mandei o Instagram da Igreja para ela conhecer.</t>
+  </si>
+  <si>
+    <t>Já havia entrado em contato com o Gabriel no dia 02/02/25. Entrei em contato novamente e me coloquei à disposição. Perguntei sobre o GC.</t>
+  </si>
+  <si>
+    <t>Orlando Gouvea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jardim Oceanico </t>
+  </si>
+  <si>
+    <t>21 99636-6685</t>
+  </si>
+  <si>
+    <t>Entrei em contato pelo WhatsApp. Falei sobre GC e dei as boas vindas</t>
+  </si>
+  <si>
+    <t>Raphael De Freitas Moreira</t>
+  </si>
+  <si>
+    <t>Taquara</t>
+  </si>
+  <si>
+    <t>21 97900-7999</t>
+  </si>
+  <si>
+    <t>Abraão Nunes Vasconcelos</t>
+  </si>
+  <si>
+    <t>21 99659-4949</t>
+  </si>
+  <si>
+    <t>Número errado.</t>
+  </si>
+  <si>
+    <t>Matheus De Góis Santos</t>
+  </si>
+  <si>
+    <t>Catumbi</t>
+  </si>
+  <si>
+    <t>21 98979-0703</t>
+  </si>
+  <si>
+    <t>Paulo Calarge Filho</t>
+  </si>
+  <si>
+    <t>21 99988-2230</t>
+  </si>
+  <si>
+    <t>Henrique Leite Santiago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vidigal </t>
+  </si>
+  <si>
+    <t>21 97876-1508</t>
+  </si>
+  <si>
+    <t>Entrei em contato pelo WhatsApp. Falei sobre GC e dei as boas vindas. Encaminhei para o líder do NEXTEEN.</t>
+  </si>
+  <si>
+    <t>11/02/2025</t>
+  </si>
+  <si>
+    <t>Felipe Gabriel</t>
+  </si>
+  <si>
+    <t>Gamboa</t>
+  </si>
+  <si>
+    <t>21 99256-1102</t>
+  </si>
+  <si>
+    <t>Entrei em contato pelo WhatsApp. Falei sobre o NEXTEEN e dei as boas vindas. Encaminhei para o líder do NEXTEEN. Disse que conhece o Gylsinho e a galera do NEXTEEN. Reforcei a necessidade de não andar sozinho.</t>
+  </si>
+  <si>
+    <t>André Silva Entre</t>
+  </si>
+  <si>
+    <t>Santa Teresa</t>
+  </si>
+  <si>
+    <t>21 97289-8303</t>
+  </si>
+  <si>
+    <t>Lierte Honorato Risperi Junior</t>
+  </si>
+  <si>
+    <t>Higienópolis</t>
+  </si>
+  <si>
+    <t>21 99992-8273</t>
+  </si>
+  <si>
+    <t>culto maximos</t>
+  </si>
+  <si>
+    <t>Noé Júnior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rocinha </t>
+  </si>
+  <si>
+    <t>21 97428-5527</t>
+  </si>
+  <si>
+    <t>Entrei em contato pelo WhatsApp. Falei sobre GC e dei as boas vindas.
+Se abriu comigo e disse que fez seminário, foi obreiro, foi diácono, frequentou a Lagoinha de BH. Pediu que eu orasse por ele e eu orei.</t>
+  </si>
+  <si>
+    <t>enviei mensagem / respondeu/ encaminhada para gc da tijuca/falei com Jena</t>
+  </si>
+  <si>
+    <t>Paloma Bastos</t>
+  </si>
+  <si>
+    <t>21 99297-8615</t>
+  </si>
+  <si>
+    <t>enviei mensagem /respondeu dizendo que gostaria de se batizar e frequentar gc. Encaminhei para Supervisora Fran.</t>
+  </si>
+  <si>
+    <t>Ana Clara Freitas</t>
+  </si>
+  <si>
+    <t>Bonsucesso</t>
+  </si>
+  <si>
+    <t>21 97875-3731</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elizabeth </t>
+  </si>
+  <si>
+    <t>21 98885-4914</t>
+  </si>
+  <si>
+    <t>Efigênia Oliveira</t>
+  </si>
+  <si>
+    <t>21 96916-9736</t>
+  </si>
+  <si>
+    <t>Patrícia Da Silva</t>
+  </si>
+  <si>
+    <t>21 99940-9926</t>
+  </si>
+  <si>
+    <t>Daniela Andrade</t>
+  </si>
+  <si>
+    <t>Pinheiros</t>
+  </si>
+  <si>
+    <t>São Paulo / SP</t>
+  </si>
+  <si>
+    <t>47 99911-4205</t>
+  </si>
+  <si>
+    <t>Julia Dias Fernandes</t>
+  </si>
+  <si>
+    <t>11 98109-1555</t>
+  </si>
+  <si>
+    <t>Rabeche Martins</t>
+  </si>
+  <si>
+    <t>São Cristóvão</t>
+  </si>
+  <si>
+    <t>21 99129-8846</t>
+  </si>
+  <si>
+    <t>Alessandra Mestre</t>
+  </si>
+  <si>
+    <t>21 99024-8229</t>
   </si>
 </sst>
 </file>
@@ -1918,11 +2106,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F662FB8-528C-4013-B4C5-67C7C16EE720}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:P135"/>
+  <dimension ref="A1:O157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A156" sqref="A156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1942,10 +2129,9 @@
     <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="130" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1991,11 +2177,8 @@
       <c r="O1" s="2" t="s">
         <v>488</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -2041,12 +2224,8 @@
       <c r="O2" t="s">
         <v>80</v>
       </c>
-      <c r="P2">
-        <f>IF(O2="Não",0,1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -2092,12 +2271,8 @@
       <c r="O3" t="s">
         <v>80</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P66" si="0">IF(O3="Não",0,1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2143,12 +2318,8 @@
       <c r="O4" t="s">
         <v>24</v>
       </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -2194,12 +2365,8 @@
       <c r="O5" t="s">
         <v>80</v>
       </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -2245,12 +2412,8 @@
       <c r="O6" t="s">
         <v>80</v>
       </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -2296,12 +2459,8 @@
       <c r="O7" t="s">
         <v>24</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -2347,12 +2506,8 @@
       <c r="O8" t="s">
         <v>24</v>
       </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -2398,12 +2553,8 @@
       <c r="O9" t="s">
         <v>80</v>
       </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2449,12 +2600,8 @@
       <c r="O10" t="s">
         <v>80</v>
       </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2500,12 +2647,8 @@
       <c r="O11" t="s">
         <v>80</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -2551,12 +2694,8 @@
       <c r="O12" t="s">
         <v>80</v>
       </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -2602,12 +2741,8 @@
       <c r="O13" t="s">
         <v>24</v>
       </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -2653,12 +2788,8 @@
       <c r="O14" t="s">
         <v>80</v>
       </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2704,12 +2835,8 @@
       <c r="O15" t="s">
         <v>80</v>
       </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2755,12 +2882,8 @@
       <c r="O16" t="s">
         <v>24</v>
       </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2806,12 +2929,8 @@
       <c r="O17" t="s">
         <v>24</v>
       </c>
-      <c r="P17">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -2857,12 +2976,8 @@
       <c r="O18" t="s">
         <v>80</v>
       </c>
-      <c r="P18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -2908,12 +3023,8 @@
       <c r="O19" t="s">
         <v>80</v>
       </c>
-      <c r="P19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -2959,12 +3070,8 @@
       <c r="O20" t="s">
         <v>24</v>
       </c>
-      <c r="P20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -3010,12 +3117,8 @@
       <c r="O21" t="s">
         <v>24</v>
       </c>
-      <c r="P21">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -3061,12 +3164,8 @@
       <c r="O22" t="s">
         <v>24</v>
       </c>
-      <c r="P22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -3112,12 +3211,8 @@
       <c r="O23" t="s">
         <v>80</v>
       </c>
-      <c r="P23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -3163,12 +3258,8 @@
       <c r="O24" t="s">
         <v>80</v>
       </c>
-      <c r="P24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -3214,12 +3305,8 @@
       <c r="O25" t="s">
         <v>80</v>
       </c>
-      <c r="P25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -3265,12 +3352,8 @@
       <c r="O26" t="s">
         <v>80</v>
       </c>
-      <c r="P26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -3316,12 +3399,8 @@
       <c r="O27" t="s">
         <v>80</v>
       </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -3367,12 +3446,8 @@
       <c r="O28" t="s">
         <v>80</v>
       </c>
-      <c r="P28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -3418,12 +3493,8 @@
       <c r="O29" t="s">
         <v>24</v>
       </c>
-      <c r="P29">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -3469,12 +3540,8 @@
       <c r="O30" t="s">
         <v>80</v>
       </c>
-      <c r="P30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -3520,12 +3587,8 @@
       <c r="O31" t="s">
         <v>80</v>
       </c>
-      <c r="P31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -3571,12 +3634,8 @@
       <c r="O32" t="s">
         <v>24</v>
       </c>
-      <c r="P32">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -3622,12 +3681,8 @@
       <c r="O33" t="s">
         <v>80</v>
       </c>
-      <c r="P33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -3673,12 +3728,8 @@
       <c r="O34" t="s">
         <v>24</v>
       </c>
-      <c r="P34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -3724,12 +3775,8 @@
       <c r="O35" t="s">
         <v>80</v>
       </c>
-      <c r="P35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -3775,12 +3822,8 @@
       <c r="O36" t="s">
         <v>80</v>
       </c>
-      <c r="P36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -3826,12 +3869,8 @@
       <c r="O37" t="s">
         <v>24</v>
       </c>
-      <c r="P37">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -3877,12 +3916,8 @@
       <c r="O38" t="s">
         <v>80</v>
       </c>
-      <c r="P38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -3928,12 +3963,8 @@
       <c r="O39" t="s">
         <v>80</v>
       </c>
-      <c r="P39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>174</v>
       </c>
@@ -3979,12 +4010,8 @@
       <c r="O40" t="s">
         <v>24</v>
       </c>
-      <c r="P40">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>174</v>
       </c>
@@ -4030,12 +4057,8 @@
       <c r="O41" t="s">
         <v>80</v>
       </c>
-      <c r="P41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>174</v>
       </c>
@@ -4081,12 +4104,8 @@
       <c r="O42" t="s">
         <v>80</v>
       </c>
-      <c r="P42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>174</v>
       </c>
@@ -4129,12 +4148,8 @@
       <c r="O43" t="s">
         <v>24</v>
       </c>
-      <c r="P43">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>174</v>
       </c>
@@ -4180,12 +4195,8 @@
       <c r="O44" t="s">
         <v>80</v>
       </c>
-      <c r="P44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>174</v>
       </c>
@@ -4231,12 +4242,8 @@
       <c r="O45" t="s">
         <v>24</v>
       </c>
-      <c r="P45">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>174</v>
       </c>
@@ -4279,12 +4286,8 @@
       <c r="O46" t="s">
         <v>80</v>
       </c>
-      <c r="P46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>174</v>
       </c>
@@ -4330,12 +4333,8 @@
       <c r="O47" t="s">
         <v>80</v>
       </c>
-      <c r="P47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>174</v>
       </c>
@@ -4381,12 +4380,8 @@
       <c r="O48" t="s">
         <v>80</v>
       </c>
-      <c r="P48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>209</v>
       </c>
@@ -4432,12 +4427,8 @@
       <c r="O49" t="s">
         <v>24</v>
       </c>
-      <c r="P49">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>209</v>
       </c>
@@ -4483,12 +4474,8 @@
       <c r="O50" t="s">
         <v>24</v>
       </c>
-      <c r="P50">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>209</v>
       </c>
@@ -4534,12 +4521,8 @@
       <c r="O51" t="s">
         <v>80</v>
       </c>
-      <c r="P51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>209</v>
       </c>
@@ -4585,12 +4568,8 @@
       <c r="O52" t="s">
         <v>24</v>
       </c>
-      <c r="P52">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>209</v>
       </c>
@@ -4636,12 +4615,8 @@
       <c r="O53" t="s">
         <v>24</v>
       </c>
-      <c r="P53">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>209</v>
       </c>
@@ -4687,12 +4662,8 @@
       <c r="O54" t="s">
         <v>80</v>
       </c>
-      <c r="P54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" ht="72" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>209</v>
       </c>
@@ -4738,12 +4709,8 @@
       <c r="O55" t="s">
         <v>24</v>
       </c>
-      <c r="P55">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>209</v>
       </c>
@@ -4789,12 +4756,8 @@
       <c r="O56" t="s">
         <v>80</v>
       </c>
-      <c r="P56">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>209</v>
       </c>
@@ -4840,12 +4803,8 @@
       <c r="O57" t="s">
         <v>24</v>
       </c>
-      <c r="P57">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>209</v>
       </c>
@@ -4891,12 +4850,8 @@
       <c r="O58" t="s">
         <v>80</v>
       </c>
-      <c r="P58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>209</v>
       </c>
@@ -4942,12 +4897,8 @@
       <c r="O59" t="s">
         <v>80</v>
       </c>
-      <c r="P59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>209</v>
       </c>
@@ -4993,12 +4944,8 @@
       <c r="O60" t="s">
         <v>24</v>
       </c>
-      <c r="P60">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>209</v>
       </c>
@@ -5044,12 +4991,8 @@
       <c r="O61" t="s">
         <v>24</v>
       </c>
-      <c r="P61">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>209</v>
       </c>
@@ -5095,12 +5038,8 @@
       <c r="O62" t="s">
         <v>24</v>
       </c>
-      <c r="P62">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>209</v>
       </c>
@@ -5146,12 +5085,8 @@
       <c r="O63" t="s">
         <v>80</v>
       </c>
-      <c r="P63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>209</v>
       </c>
@@ -5197,12 +5132,8 @@
       <c r="O64" t="s">
         <v>80</v>
       </c>
-      <c r="P64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>209</v>
       </c>
@@ -5248,12 +5179,8 @@
       <c r="O65" t="s">
         <v>24</v>
       </c>
-      <c r="P65">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>209</v>
       </c>
@@ -5299,12 +5226,8 @@
       <c r="O66" t="s">
         <v>80</v>
       </c>
-      <c r="P66">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>209</v>
       </c>
@@ -5350,12 +5273,8 @@
       <c r="O67" t="s">
         <v>24</v>
       </c>
-      <c r="P67">
-        <f t="shared" ref="P67:P130" si="1">IF(O67="Não",0,1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>209</v>
       </c>
@@ -5401,12 +5320,8 @@
       <c r="O68" t="s">
         <v>80</v>
       </c>
-      <c r="P68">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>209</v>
       </c>
@@ -5452,12 +5367,8 @@
       <c r="O69" t="s">
         <v>24</v>
       </c>
-      <c r="P69">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>209</v>
       </c>
@@ -5503,12 +5414,8 @@
       <c r="O70" t="s">
         <v>80</v>
       </c>
-      <c r="P70">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>209</v>
       </c>
@@ -5554,12 +5461,8 @@
       <c r="O71" t="s">
         <v>24</v>
       </c>
-      <c r="P71">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>209</v>
       </c>
@@ -5605,12 +5508,8 @@
       <c r="O72" t="s">
         <v>80</v>
       </c>
-      <c r="P72">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>295</v>
       </c>
@@ -5656,12 +5555,8 @@
       <c r="O73" t="s">
         <v>24</v>
       </c>
-      <c r="P73">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>295</v>
       </c>
@@ -5707,12 +5602,8 @@
       <c r="O74" t="s">
         <v>80</v>
       </c>
-      <c r="P74">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>295</v>
       </c>
@@ -5758,12 +5649,8 @@
       <c r="O75" t="s">
         <v>24</v>
       </c>
-      <c r="P75">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>295</v>
       </c>
@@ -5809,12 +5696,8 @@
       <c r="O76" t="s">
         <v>24</v>
       </c>
-      <c r="P76">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>295</v>
       </c>
@@ -5860,12 +5743,8 @@
       <c r="O77" t="s">
         <v>80</v>
       </c>
-      <c r="P77">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>295</v>
       </c>
@@ -5911,12 +5790,8 @@
       <c r="O78" t="s">
         <v>80</v>
       </c>
-      <c r="P78">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>295</v>
       </c>
@@ -5962,12 +5837,8 @@
       <c r="O79" t="s">
         <v>24</v>
       </c>
-      <c r="P79">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>295</v>
       </c>
@@ -6013,12 +5884,8 @@
       <c r="O80" t="s">
         <v>80</v>
       </c>
-      <c r="P80">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>295</v>
       </c>
@@ -6064,12 +5931,8 @@
       <c r="O81" t="s">
         <v>80</v>
       </c>
-      <c r="P81">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>295</v>
       </c>
@@ -6115,12 +5978,8 @@
       <c r="O82" t="s">
         <v>24</v>
       </c>
-      <c r="P82">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>295</v>
       </c>
@@ -6166,12 +6025,8 @@
       <c r="O83" t="s">
         <v>24</v>
       </c>
-      <c r="P83">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>295</v>
       </c>
@@ -6217,12 +6072,8 @@
       <c r="O84" t="s">
         <v>24</v>
       </c>
-      <c r="P84">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>295</v>
       </c>
@@ -6268,12 +6119,8 @@
       <c r="O85" t="s">
         <v>24</v>
       </c>
-      <c r="P85">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>295</v>
       </c>
@@ -6319,12 +6166,8 @@
       <c r="O86" t="s">
         <v>80</v>
       </c>
-      <c r="P86">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>295</v>
       </c>
@@ -6370,12 +6213,8 @@
       <c r="O87" t="s">
         <v>24</v>
       </c>
-      <c r="P87">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>348</v>
       </c>
@@ -6421,12 +6260,8 @@
       <c r="O88" t="s">
         <v>80</v>
       </c>
-      <c r="P88">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>349</v>
       </c>
@@ -6472,12 +6307,8 @@
       <c r="O89" t="s">
         <v>80</v>
       </c>
-      <c r="P89">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>349</v>
       </c>
@@ -6523,12 +6354,8 @@
       <c r="O90" t="s">
         <v>80</v>
       </c>
-      <c r="P90">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>349</v>
       </c>
@@ -6574,12 +6401,8 @@
       <c r="O91" t="s">
         <v>24</v>
       </c>
-      <c r="P91">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>349</v>
       </c>
@@ -6625,12 +6448,8 @@
       <c r="O92" t="s">
         <v>24</v>
       </c>
-      <c r="P92">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>349</v>
       </c>
@@ -6676,12 +6495,8 @@
       <c r="O93" t="s">
         <v>24</v>
       </c>
-      <c r="P93">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>349</v>
       </c>
@@ -6727,12 +6542,8 @@
       <c r="O94" t="s">
         <v>24</v>
       </c>
-      <c r="P94">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>349</v>
       </c>
@@ -6778,12 +6589,8 @@
       <c r="O95" t="s">
         <v>80</v>
       </c>
-      <c r="P95">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>350</v>
       </c>
@@ -6829,12 +6636,8 @@
       <c r="O96" t="s">
         <v>24</v>
       </c>
-      <c r="P96">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>350</v>
       </c>
@@ -6880,12 +6683,8 @@
       <c r="O97" t="s">
         <v>24</v>
       </c>
-      <c r="P97">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>350</v>
       </c>
@@ -6931,12 +6730,8 @@
       <c r="O98" t="s">
         <v>24</v>
       </c>
-      <c r="P98">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>350</v>
       </c>
@@ -6982,12 +6777,8 @@
       <c r="O99" t="s">
         <v>24</v>
       </c>
-      <c r="P99">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>350</v>
       </c>
@@ -7033,12 +6824,8 @@
       <c r="O100" t="s">
         <v>24</v>
       </c>
-      <c r="P100">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>350</v>
       </c>
@@ -7084,12 +6871,8 @@
       <c r="O101" t="s">
         <v>24</v>
       </c>
-      <c r="P101">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>348</v>
       </c>
@@ -7135,12 +6918,8 @@
       <c r="O102" t="s">
         <v>24</v>
       </c>
-      <c r="P102">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>348</v>
       </c>
@@ -7186,12 +6965,8 @@
       <c r="O103" t="s">
         <v>80</v>
       </c>
-      <c r="P103">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>349</v>
       </c>
@@ -7237,12 +7012,8 @@
       <c r="O104" t="s">
         <v>80</v>
       </c>
-      <c r="P104">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>349</v>
       </c>
@@ -7288,12 +7059,8 @@
       <c r="O105" t="s">
         <v>80</v>
       </c>
-      <c r="P105">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>349</v>
       </c>
@@ -7339,12 +7106,8 @@
       <c r="O106" t="s">
         <v>80</v>
       </c>
-      <c r="P106">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>349</v>
       </c>
@@ -7390,12 +7153,8 @@
       <c r="O107" t="s">
         <v>80</v>
       </c>
-      <c r="P107">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>349</v>
       </c>
@@ -7441,12 +7200,8 @@
       <c r="O108" t="s">
         <v>24</v>
       </c>
-      <c r="P108">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>349</v>
       </c>
@@ -7492,12 +7247,8 @@
       <c r="O109" t="s">
         <v>24</v>
       </c>
-      <c r="P109">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>349</v>
       </c>
@@ -7543,12 +7294,8 @@
       <c r="O110" t="s">
         <v>80</v>
       </c>
-      <c r="P110">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>349</v>
       </c>
@@ -7594,12 +7341,8 @@
       <c r="O111" t="s">
         <v>80</v>
       </c>
-      <c r="P111">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>349</v>
       </c>
@@ -7645,12 +7388,8 @@
       <c r="O112" t="s">
         <v>24</v>
       </c>
-      <c r="P112">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>349</v>
       </c>
@@ -7696,12 +7435,8 @@
       <c r="O113" t="s">
         <v>80</v>
       </c>
-      <c r="P113">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>349</v>
       </c>
@@ -7747,12 +7482,8 @@
       <c r="O114" t="s">
         <v>80</v>
       </c>
-      <c r="P114">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>349</v>
       </c>
@@ -7798,12 +7529,8 @@
       <c r="O115" t="s">
         <v>24</v>
       </c>
-      <c r="P115">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>349</v>
       </c>
@@ -7849,12 +7576,8 @@
       <c r="O116" t="s">
         <v>80</v>
       </c>
-      <c r="P116">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>349</v>
       </c>
@@ -7900,12 +7623,8 @@
       <c r="O117" t="s">
         <v>24</v>
       </c>
-      <c r="P117">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>349</v>
       </c>
@@ -7951,12 +7670,8 @@
       <c r="O118" t="s">
         <v>24</v>
       </c>
-      <c r="P118">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>349</v>
       </c>
@@ -8002,12 +7717,8 @@
       <c r="O119" t="s">
         <v>24</v>
       </c>
-      <c r="P119">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="120" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>349</v>
       </c>
@@ -8053,12 +7764,8 @@
       <c r="O120" t="s">
         <v>80</v>
       </c>
-      <c r="P120">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>349</v>
       </c>
@@ -8104,12 +7811,8 @@
       <c r="O121" t="s">
         <v>80</v>
       </c>
-      <c r="P121">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>349</v>
       </c>
@@ -8155,12 +7858,8 @@
       <c r="O122" t="s">
         <v>80</v>
       </c>
-      <c r="P122">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="123" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>349</v>
       </c>
@@ -8206,12 +7905,8 @@
       <c r="O123" t="s">
         <v>80</v>
       </c>
-      <c r="P123">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="124" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>349</v>
       </c>
@@ -8257,12 +7952,8 @@
       <c r="O124" t="s">
         <v>80</v>
       </c>
-      <c r="P124">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="125" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>349</v>
       </c>
@@ -8308,12 +7999,8 @@
       <c r="O125" t="s">
         <v>80</v>
       </c>
-      <c r="P125">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="126" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>349</v>
       </c>
@@ -8359,12 +8046,8 @@
       <c r="O126" t="s">
         <v>80</v>
       </c>
-      <c r="P126">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="127" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>350</v>
       </c>
@@ -8410,12 +8093,8 @@
       <c r="O127" t="s">
         <v>80</v>
       </c>
-      <c r="P127">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>350</v>
       </c>
@@ -8461,12 +8140,8 @@
       <c r="O128" t="s">
         <v>80</v>
       </c>
-      <c r="P128">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>350</v>
       </c>
@@ -8512,12 +8187,8 @@
       <c r="O129" t="s">
         <v>24</v>
       </c>
-      <c r="P129">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>350</v>
       </c>
@@ -8563,12 +8234,8 @@
       <c r="O130" t="s">
         <v>80</v>
       </c>
-      <c r="P130">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>350</v>
       </c>
@@ -8614,12 +8281,8 @@
       <c r="O131" t="s">
         <v>80</v>
       </c>
-      <c r="P131">
-        <f t="shared" ref="P131:P135" si="2">IF(O131="Não",0,1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>350</v>
       </c>
@@ -8665,12 +8328,8 @@
       <c r="O132" t="s">
         <v>24</v>
       </c>
-      <c r="P132">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>350</v>
       </c>
@@ -8716,12 +8375,8 @@
       <c r="O133" t="s">
         <v>24</v>
       </c>
-      <c r="P133">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>350</v>
       </c>
@@ -8764,12 +8419,8 @@
       <c r="O134" t="s">
         <v>80</v>
       </c>
-      <c r="P134">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:16" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="135" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>476</v>
       </c>
@@ -8812,19 +8463,1042 @@
       <c r="O135" t="s">
         <v>80</v>
       </c>
-      <c r="P135">
-        <f t="shared" si="2"/>
-        <v>0</v>
+    </row>
+    <row r="136" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>476</v>
+      </c>
+      <c r="B136" t="s">
+        <v>40</v>
+      </c>
+      <c r="C136" t="s">
+        <v>27</v>
+      </c>
+      <c r="D136" t="s">
+        <v>489</v>
+      </c>
+      <c r="E136" t="s">
+        <v>18</v>
+      </c>
+      <c r="F136" t="s">
+        <v>29</v>
+      </c>
+      <c r="G136">
+        <v>48</v>
+      </c>
+      <c r="H136" t="s">
+        <v>129</v>
+      </c>
+      <c r="I136" t="s">
+        <v>22</v>
+      </c>
+      <c r="J136" t="s">
+        <v>490</v>
+      </c>
+      <c r="K136" t="s">
+        <v>24</v>
+      </c>
+      <c r="L136" t="s">
+        <v>25</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N136" t="s">
+        <v>491</v>
+      </c>
+      <c r="O136" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="137" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>476</v>
+      </c>
+      <c r="B137" t="s">
+        <v>40</v>
+      </c>
+      <c r="C137" t="s">
+        <v>41</v>
+      </c>
+      <c r="D137" t="s">
+        <v>296</v>
+      </c>
+      <c r="E137" t="s">
+        <v>18</v>
+      </c>
+      <c r="F137" t="s">
+        <v>29</v>
+      </c>
+      <c r="G137">
+        <v>22</v>
+      </c>
+      <c r="H137" t="s">
+        <v>297</v>
+      </c>
+      <c r="I137" t="s">
+        <v>22</v>
+      </c>
+      <c r="J137" t="s">
+        <v>298</v>
+      </c>
+      <c r="K137" t="s">
+        <v>24</v>
+      </c>
+      <c r="L137" t="s">
+        <v>46</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N137" t="s">
+        <v>492</v>
+      </c>
+      <c r="O137" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="138" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>476</v>
+      </c>
+      <c r="B138" t="s">
+        <v>40</v>
+      </c>
+      <c r="C138" t="s">
+        <v>16</v>
+      </c>
+      <c r="D138" t="s">
+        <v>493</v>
+      </c>
+      <c r="E138" t="s">
+        <v>18</v>
+      </c>
+      <c r="F138" t="s">
+        <v>58</v>
+      </c>
+      <c r="G138">
+        <v>58</v>
+      </c>
+      <c r="H138" t="s">
+        <v>494</v>
+      </c>
+      <c r="I138" t="s">
+        <v>36</v>
+      </c>
+      <c r="J138" t="s">
+        <v>495</v>
+      </c>
+      <c r="K138" t="s">
+        <v>24</v>
+      </c>
+      <c r="L138" t="s">
+        <v>25</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="N138" t="s">
+        <v>496</v>
+      </c>
+      <c r="O138" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="139" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>476</v>
+      </c>
+      <c r="B139" t="s">
+        <v>40</v>
+      </c>
+      <c r="C139" t="s">
+        <v>41</v>
+      </c>
+      <c r="D139" t="s">
+        <v>497</v>
+      </c>
+      <c r="E139" t="s">
+        <v>18</v>
+      </c>
+      <c r="F139" t="s">
+        <v>29</v>
+      </c>
+      <c r="G139">
+        <v>40</v>
+      </c>
+      <c r="H139" t="s">
+        <v>498</v>
+      </c>
+      <c r="I139" t="s">
+        <v>22</v>
+      </c>
+      <c r="J139" t="s">
+        <v>499</v>
+      </c>
+      <c r="K139" t="s">
+        <v>24</v>
+      </c>
+      <c r="L139" t="s">
+        <v>25</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N139" t="s">
+        <v>496</v>
+      </c>
+      <c r="O139" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>476</v>
+      </c>
+      <c r="B140" t="s">
+        <v>40</v>
+      </c>
+      <c r="C140" t="s">
+        <v>41</v>
+      </c>
+      <c r="D140" t="s">
+        <v>500</v>
+      </c>
+      <c r="E140" t="s">
+        <v>18</v>
+      </c>
+      <c r="F140" t="s">
+        <v>29</v>
+      </c>
+      <c r="G140">
+        <v>20</v>
+      </c>
+      <c r="H140" t="s">
+        <v>44</v>
+      </c>
+      <c r="I140" t="s">
+        <v>22</v>
+      </c>
+      <c r="J140" t="s">
+        <v>501</v>
+      </c>
+      <c r="K140" t="s">
+        <v>24</v>
+      </c>
+      <c r="L140" t="s">
+        <v>25</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N140" t="s">
+        <v>502</v>
+      </c>
+      <c r="O140" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="141" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>476</v>
+      </c>
+      <c r="B141" t="s">
+        <v>40</v>
+      </c>
+      <c r="C141" t="s">
+        <v>41</v>
+      </c>
+      <c r="D141" t="s">
+        <v>503</v>
+      </c>
+      <c r="E141" t="s">
+        <v>18</v>
+      </c>
+      <c r="F141" t="s">
+        <v>29</v>
+      </c>
+      <c r="G141">
+        <v>26</v>
+      </c>
+      <c r="H141" t="s">
+        <v>504</v>
+      </c>
+      <c r="I141" t="s">
+        <v>22</v>
+      </c>
+      <c r="J141" t="s">
+        <v>505</v>
+      </c>
+      <c r="K141" t="s">
+        <v>24</v>
+      </c>
+      <c r="L141" t="s">
+        <v>46</v>
+      </c>
+      <c r="M141" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N141" t="s">
+        <v>496</v>
+      </c>
+      <c r="O141" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="142" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>476</v>
+      </c>
+      <c r="B142" t="s">
+        <v>40</v>
+      </c>
+      <c r="C142" t="s">
+        <v>27</v>
+      </c>
+      <c r="D142" t="s">
+        <v>506</v>
+      </c>
+      <c r="E142" t="s">
+        <v>18</v>
+      </c>
+      <c r="F142" t="s">
+        <v>91</v>
+      </c>
+      <c r="G142">
+        <v>60</v>
+      </c>
+      <c r="H142" t="s">
+        <v>297</v>
+      </c>
+      <c r="I142" t="s">
+        <v>22</v>
+      </c>
+      <c r="J142" t="s">
+        <v>507</v>
+      </c>
+      <c r="K142" t="s">
+        <v>24</v>
+      </c>
+      <c r="L142" t="s">
+        <v>25</v>
+      </c>
+      <c r="M142" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N142" t="s">
+        <v>496</v>
+      </c>
+      <c r="O142" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="143" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>476</v>
+      </c>
+      <c r="B143" t="s">
+        <v>40</v>
+      </c>
+      <c r="C143" t="s">
+        <v>27</v>
+      </c>
+      <c r="D143" t="s">
+        <v>508</v>
+      </c>
+      <c r="E143" t="s">
+        <v>18</v>
+      </c>
+      <c r="F143" t="s">
+        <v>29</v>
+      </c>
+      <c r="G143">
+        <v>15</v>
+      </c>
+      <c r="H143" t="s">
+        <v>509</v>
+      </c>
+      <c r="I143" t="s">
+        <v>158</v>
+      </c>
+      <c r="J143" t="s">
+        <v>510</v>
+      </c>
+      <c r="K143" t="s">
+        <v>24</v>
+      </c>
+      <c r="L143" t="s">
+        <v>25</v>
+      </c>
+      <c r="M143" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N143" t="s">
+        <v>511</v>
+      </c>
+      <c r="O143" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="144" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>512</v>
+      </c>
+      <c r="B144" t="s">
+        <v>58</v>
+      </c>
+      <c r="C144" t="s">
+        <v>41</v>
+      </c>
+      <c r="D144" t="s">
+        <v>513</v>
+      </c>
+      <c r="E144" t="s">
+        <v>18</v>
+      </c>
+      <c r="F144" t="s">
+        <v>29</v>
+      </c>
+      <c r="G144">
+        <v>17</v>
+      </c>
+      <c r="H144" t="s">
+        <v>514</v>
+      </c>
+      <c r="I144" t="s">
+        <v>22</v>
+      </c>
+      <c r="J144" t="s">
+        <v>515</v>
+      </c>
+      <c r="K144" t="s">
+        <v>24</v>
+      </c>
+      <c r="L144" t="s">
+        <v>25</v>
+      </c>
+      <c r="M144" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N144" t="s">
+        <v>516</v>
+      </c>
+      <c r="O144" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>512</v>
+      </c>
+      <c r="B145" t="s">
+        <v>58</v>
+      </c>
+      <c r="C145" t="s">
+        <v>41</v>
+      </c>
+      <c r="D145" t="s">
+        <v>517</v>
+      </c>
+      <c r="E145" t="s">
+        <v>18</v>
+      </c>
+      <c r="F145" t="s">
+        <v>19</v>
+      </c>
+      <c r="G145">
+        <v>44</v>
+      </c>
+      <c r="H145" t="s">
+        <v>518</v>
+      </c>
+      <c r="I145" t="s">
+        <v>22</v>
+      </c>
+      <c r="J145" t="s">
+        <v>519</v>
+      </c>
+      <c r="K145" t="s">
+        <v>24</v>
+      </c>
+      <c r="L145" t="s">
+        <v>46</v>
+      </c>
+      <c r="M145" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N145" t="s">
+        <v>496</v>
+      </c>
+      <c r="O145" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="146" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>512</v>
+      </c>
+      <c r="B146" t="s">
+        <v>58</v>
+      </c>
+      <c r="C146" t="s">
+        <v>16</v>
+      </c>
+      <c r="D146" t="s">
+        <v>520</v>
+      </c>
+      <c r="E146" t="s">
+        <v>18</v>
+      </c>
+      <c r="F146" t="s">
+        <v>29</v>
+      </c>
+      <c r="G146">
+        <v>39</v>
+      </c>
+      <c r="H146" t="s">
+        <v>521</v>
+      </c>
+      <c r="I146" t="s">
+        <v>22</v>
+      </c>
+      <c r="J146" t="s">
+        <v>522</v>
+      </c>
+      <c r="K146" t="s">
+        <v>24</v>
+      </c>
+      <c r="L146" t="s">
+        <v>25</v>
+      </c>
+      <c r="M146" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N146" t="s">
+        <v>496</v>
+      </c>
+      <c r="O146" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>512</v>
+      </c>
+      <c r="B147" t="s">
+        <v>523</v>
+      </c>
+      <c r="C147" t="s">
+        <v>41</v>
+      </c>
+      <c r="D147" t="s">
+        <v>524</v>
+      </c>
+      <c r="E147" t="s">
+        <v>18</v>
+      </c>
+      <c r="F147" t="s">
+        <v>29</v>
+      </c>
+      <c r="G147">
+        <v>32</v>
+      </c>
+      <c r="H147" t="s">
+        <v>525</v>
+      </c>
+      <c r="I147" t="s">
+        <v>158</v>
+      </c>
+      <c r="J147" t="s">
+        <v>526</v>
+      </c>
+      <c r="K147" t="s">
+        <v>24</v>
+      </c>
+      <c r="L147" t="s">
+        <v>202</v>
+      </c>
+      <c r="M147" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N147" t="s">
+        <v>527</v>
+      </c>
+      <c r="O147" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>476</v>
+      </c>
+      <c r="B148" t="s">
+        <v>40</v>
+      </c>
+      <c r="C148" t="s">
+        <v>41</v>
+      </c>
+      <c r="D148" t="s">
+        <v>477</v>
+      </c>
+      <c r="E148" t="s">
+        <v>65</v>
+      </c>
+      <c r="F148" t="s">
+        <v>91</v>
+      </c>
+      <c r="G148">
+        <v>35</v>
+      </c>
+      <c r="H148" t="s">
+        <v>21</v>
+      </c>
+      <c r="I148" t="s">
+        <v>22</v>
+      </c>
+      <c r="J148" t="s">
+        <v>478</v>
+      </c>
+      <c r="K148" t="s">
+        <v>24</v>
+      </c>
+      <c r="L148" t="s">
+        <v>25</v>
+      </c>
+      <c r="M148" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N148" t="s">
+        <v>528</v>
+      </c>
+      <c r="O148" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
+        <v>476</v>
+      </c>
+      <c r="B149" t="s">
+        <v>40</v>
+      </c>
+      <c r="C149" t="s">
+        <v>27</v>
+      </c>
+      <c r="D149" t="s">
+        <v>529</v>
+      </c>
+      <c r="E149" t="s">
+        <v>65</v>
+      </c>
+      <c r="F149" t="s">
+        <v>19</v>
+      </c>
+      <c r="G149">
+        <v>39</v>
+      </c>
+      <c r="H149" t="s">
+        <v>44</v>
+      </c>
+      <c r="I149" t="s">
+        <v>22</v>
+      </c>
+      <c r="J149" t="s">
+        <v>530</v>
+      </c>
+      <c r="K149" t="s">
+        <v>24</v>
+      </c>
+      <c r="L149" t="s">
+        <v>202</v>
+      </c>
+      <c r="M149" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N149" t="s">
+        <v>531</v>
+      </c>
+      <c r="O149" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
+        <v>476</v>
+      </c>
+      <c r="B150" t="s">
+        <v>58</v>
+      </c>
+      <c r="C150" t="s">
+        <v>27</v>
+      </c>
+      <c r="D150" t="s">
+        <v>532</v>
+      </c>
+      <c r="E150" t="s">
+        <v>65</v>
+      </c>
+      <c r="F150" t="s">
+        <v>29</v>
+      </c>
+      <c r="G150">
+        <v>26</v>
+      </c>
+      <c r="H150" t="s">
+        <v>533</v>
+      </c>
+      <c r="I150" t="s">
+        <v>22</v>
+      </c>
+      <c r="J150" t="s">
+        <v>534</v>
+      </c>
+      <c r="K150" t="s">
+        <v>24</v>
+      </c>
+      <c r="L150" t="s">
+        <v>25</v>
+      </c>
+      <c r="M150" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N150" t="s">
+        <v>335</v>
+      </c>
+      <c r="O150" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
+        <v>476</v>
+      </c>
+      <c r="B151" t="s">
+        <v>58</v>
+      </c>
+      <c r="C151" t="s">
+        <v>41</v>
+      </c>
+      <c r="D151" t="s">
+        <v>535</v>
+      </c>
+      <c r="E151" t="s">
+        <v>65</v>
+      </c>
+      <c r="F151" t="s">
+        <v>91</v>
+      </c>
+      <c r="G151">
+        <v>63</v>
+      </c>
+      <c r="H151" t="s">
+        <v>167</v>
+      </c>
+      <c r="I151" t="s">
+        <v>22</v>
+      </c>
+      <c r="J151" t="s">
+        <v>536</v>
+      </c>
+      <c r="K151" t="s">
+        <v>24</v>
+      </c>
+      <c r="L151" t="s">
+        <v>25</v>
+      </c>
+      <c r="M151" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N151" t="s">
+        <v>280</v>
+      </c>
+      <c r="O151" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="152" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
+        <v>476</v>
+      </c>
+      <c r="B152" t="s">
+        <v>40</v>
+      </c>
+      <c r="C152" t="s">
+        <v>27</v>
+      </c>
+      <c r="D152" t="s">
+        <v>537</v>
+      </c>
+      <c r="E152" t="s">
+        <v>65</v>
+      </c>
+      <c r="F152" t="s">
+        <v>29</v>
+      </c>
+      <c r="G152">
+        <v>39</v>
+      </c>
+      <c r="H152" t="s">
+        <v>44</v>
+      </c>
+      <c r="I152" t="s">
+        <v>22</v>
+      </c>
+      <c r="J152" t="s">
+        <v>538</v>
+      </c>
+      <c r="K152" t="s">
+        <v>24</v>
+      </c>
+      <c r="L152" t="s">
+        <v>25</v>
+      </c>
+      <c r="M152" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N152" t="s">
+        <v>280</v>
+      </c>
+      <c r="O152" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="153" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A153" t="s">
+        <v>476</v>
+      </c>
+      <c r="B153" t="s">
+        <v>40</v>
+      </c>
+      <c r="C153" t="s">
+        <v>27</v>
+      </c>
+      <c r="D153" t="s">
+        <v>539</v>
+      </c>
+      <c r="E153" t="s">
+        <v>65</v>
+      </c>
+      <c r="F153" t="s">
+        <v>29</v>
+      </c>
+      <c r="G153">
+        <v>45</v>
+      </c>
+      <c r="H153" t="s">
+        <v>533</v>
+      </c>
+      <c r="I153" t="s">
+        <v>22</v>
+      </c>
+      <c r="J153" t="s">
+        <v>540</v>
+      </c>
+      <c r="K153" t="s">
+        <v>24</v>
+      </c>
+      <c r="L153" t="s">
+        <v>25</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N153" t="s">
+        <v>241</v>
+      </c>
+      <c r="O153" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
+        <v>476</v>
+      </c>
+      <c r="B154" t="s">
+        <v>40</v>
+      </c>
+      <c r="C154" t="s">
+        <v>41</v>
+      </c>
+      <c r="D154" t="s">
+        <v>541</v>
+      </c>
+      <c r="E154" t="s">
+        <v>65</v>
+      </c>
+      <c r="F154" t="s">
+        <v>29</v>
+      </c>
+      <c r="G154">
+        <v>33</v>
+      </c>
+      <c r="H154" t="s">
+        <v>542</v>
+      </c>
+      <c r="I154" t="s">
+        <v>543</v>
+      </c>
+      <c r="J154" t="s">
+        <v>544</v>
+      </c>
+      <c r="K154" t="s">
+        <v>24</v>
+      </c>
+      <c r="L154" t="s">
+        <v>25</v>
+      </c>
+      <c r="M154" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N154" t="s">
+        <v>280</v>
+      </c>
+      <c r="O154" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="155" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
+        <v>512</v>
+      </c>
+      <c r="B155" t="s">
+        <v>58</v>
+      </c>
+      <c r="C155" t="s">
+        <v>27</v>
+      </c>
+      <c r="D155" t="s">
+        <v>545</v>
+      </c>
+      <c r="E155" t="s">
+        <v>65</v>
+      </c>
+      <c r="F155" t="s">
+        <v>29</v>
+      </c>
+      <c r="G155">
+        <v>32</v>
+      </c>
+      <c r="H155" t="s">
+        <v>179</v>
+      </c>
+      <c r="I155" t="s">
+        <v>22</v>
+      </c>
+      <c r="J155" t="s">
+        <v>546</v>
+      </c>
+      <c r="K155" t="s">
+        <v>24</v>
+      </c>
+      <c r="L155" t="s">
+        <v>25</v>
+      </c>
+      <c r="M155" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N155" t="s">
+        <v>280</v>
+      </c>
+      <c r="O155" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="156" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>512</v>
+      </c>
+      <c r="B156" t="s">
+        <v>58</v>
+      </c>
+      <c r="C156" t="s">
+        <v>41</v>
+      </c>
+      <c r="D156" t="s">
+        <v>547</v>
+      </c>
+      <c r="E156" t="s">
+        <v>65</v>
+      </c>
+      <c r="F156" t="s">
+        <v>29</v>
+      </c>
+      <c r="G156">
+        <v>26</v>
+      </c>
+      <c r="H156" t="s">
+        <v>548</v>
+      </c>
+      <c r="I156" t="s">
+        <v>22</v>
+      </c>
+      <c r="J156" t="s">
+        <v>549</v>
+      </c>
+      <c r="K156" t="s">
+        <v>24</v>
+      </c>
+      <c r="L156" t="s">
+        <v>25</v>
+      </c>
+      <c r="M156" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N156" t="s">
+        <v>280</v>
+      </c>
+      <c r="O156" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="157" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>512</v>
+      </c>
+      <c r="B157" t="s">
+        <v>58</v>
+      </c>
+      <c r="C157" t="s">
+        <v>41</v>
+      </c>
+      <c r="D157" t="s">
+        <v>550</v>
+      </c>
+      <c r="E157" t="s">
+        <v>65</v>
+      </c>
+      <c r="F157" t="s">
+        <v>19</v>
+      </c>
+      <c r="G157">
+        <v>44</v>
+      </c>
+      <c r="H157" t="s">
+        <v>518</v>
+      </c>
+      <c r="I157" t="s">
+        <v>22</v>
+      </c>
+      <c r="J157" t="s">
+        <v>551</v>
+      </c>
+      <c r="K157" t="s">
+        <v>24</v>
+      </c>
+      <c r="L157" t="s">
+        <v>25</v>
+      </c>
+      <c r="M157" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N157" t="s">
+        <v>335</v>
+      </c>
+      <c r="O157" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P135" xr:uid="{2F662FB8-528C-4013-B4C5-67C7C16EE720}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="--"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Arquivo de dados atualizado
</commit_message>
<xml_diff>
--- a/Consolidado_Bridge_2025.xlsx
+++ b/Consolidado_Bridge_2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/08d87aadaabdc2cb/Desktop/BRIDGE/consolidado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="299" documentId="8_{C607EACA-C650-4A5E-95C7-07DDA7668303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F128272C-0C7D-4BF6-8DE8-F5EDD361F868}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="8_{C607EACA-C650-4A5E-95C7-07DDA7668303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96C474DF-5B0B-44C7-91AA-E638F74B5780}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EEFB68E0-0739-433A-A945-0FEA615287DD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2581" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3112" uniqueCount="758">
   <si>
     <t>Quando</t>
   </si>
@@ -1982,6 +1982,357 @@
   </si>
   <si>
     <t>21 98905-0813</t>
+  </si>
+  <si>
+    <t>Gabriele Matos</t>
+  </si>
+  <si>
+    <t>21 97301-8198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILLENA - Enviamos para Caxias pois mora lá </t>
+  </si>
+  <si>
+    <t>Tatiane Barbosa</t>
+  </si>
+  <si>
+    <t>Alcântara</t>
+  </si>
+  <si>
+    <t>São Gonçalo / RJ</t>
+  </si>
+  <si>
+    <t>21 98001-8608</t>
+  </si>
+  <si>
+    <t>MILLENA - enviei mensagem e ainda não respondeu</t>
+  </si>
+  <si>
+    <t>Mariah Eduarda De Souza Ferreira</t>
+  </si>
+  <si>
+    <t>21 98167-7603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILLENA - estamos tentando encaminhar para gc universitario. Quer apresentar a filha na igreja. </t>
+  </si>
+  <si>
+    <t>Juliana Fernandes Martins</t>
+  </si>
+  <si>
+    <t>21 99105-7547</t>
+  </si>
+  <si>
+    <t>MILLENA - encaminhada para GC na rocinha</t>
+  </si>
+  <si>
+    <t>Helen Silva</t>
+  </si>
+  <si>
+    <t>Andaraí</t>
+  </si>
+  <si>
+    <t>21 97984-3925</t>
+  </si>
+  <si>
+    <t>Thaisa Figueiredo Cardoso</t>
+  </si>
+  <si>
+    <t>Praça Da Bandeira</t>
+  </si>
+  <si>
+    <t>21 96980-9940</t>
+  </si>
+  <si>
+    <t>MILLENA</t>
+  </si>
+  <si>
+    <t>Laura Cardoso Alcantara</t>
+  </si>
+  <si>
+    <t>21 99945-5548</t>
+  </si>
+  <si>
+    <t>Artemísia Nunes</t>
+  </si>
+  <si>
+    <t>Urca</t>
+  </si>
+  <si>
+    <t>21 96559-0610</t>
+  </si>
+  <si>
+    <t>Luiza Lorenzoni Grillo</t>
+  </si>
+  <si>
+    <t>28 99986-1650</t>
+  </si>
+  <si>
+    <t>Letícia Da Silva Petronilho</t>
+  </si>
+  <si>
+    <t>21 98491-2875</t>
+  </si>
+  <si>
+    <t>Elizabeth Gracie</t>
+  </si>
+  <si>
+    <t>21 99929-6916</t>
+  </si>
+  <si>
+    <t>ENVIEI MENSAGEM/respondeu dizendo que mora ao lado da igreja e que gostaria de ir a um gc. Encaminhei para a Rajana</t>
+  </si>
+  <si>
+    <t>Juliana Pires</t>
+  </si>
+  <si>
+    <t>Rio De Ja  / --</t>
+  </si>
+  <si>
+    <t>21 97549-6257</t>
+  </si>
+  <si>
+    <t>ENVIEI MENSAGEM/ respondeu que tem interesse em um gc de casais/ encaminhada para Maryliz</t>
+  </si>
+  <si>
+    <t>Fabiana Martins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leblon </t>
+  </si>
+  <si>
+    <t>21 98310-3333</t>
+  </si>
+  <si>
+    <t>ENVIEI MENSAGEM/ respondeu dizendo que gostaria de um gc no leblon. Passei o contato para a Rajana.</t>
+  </si>
+  <si>
+    <t>Amanda Fernandes</t>
+  </si>
+  <si>
+    <t>Barra Mansa  / --</t>
+  </si>
+  <si>
+    <t>24 98862-7531</t>
+  </si>
+  <si>
+    <t>NÃO TEM WHATS</t>
+  </si>
+  <si>
+    <t>Vitória Ferreira</t>
+  </si>
+  <si>
+    <t>21 97525-3428</t>
+  </si>
+  <si>
+    <t>ENVIEI MENSAGEM / respondeu que já é da igreja e esta no gc de copacabana</t>
+  </si>
+  <si>
+    <t>Kamille Cristina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xerem </t>
+  </si>
+  <si>
+    <t>Duque De Caxias  / RJ</t>
+  </si>
+  <si>
+    <t>21 98506-8576</t>
+  </si>
+  <si>
+    <t>ENVIEI MENSAGEM</t>
+  </si>
+  <si>
+    <t>Simone Santos</t>
+  </si>
+  <si>
+    <t>11 95375-9035</t>
+  </si>
+  <si>
+    <t>Carla Andrade Pontes</t>
+  </si>
+  <si>
+    <t>21 99627-7834</t>
+  </si>
+  <si>
+    <t>encaminhada para gc mães /Rajana</t>
+  </si>
+  <si>
+    <t>Tatiana Fiche</t>
+  </si>
+  <si>
+    <t>São Conrado</t>
+  </si>
+  <si>
+    <t>Rio  / --</t>
+  </si>
+  <si>
+    <t>31 99391-0889</t>
+  </si>
+  <si>
+    <t>ENVIEI MENSAGEM/ respondeu interessada em ir ao gc/ encaminhada para Rajana</t>
+  </si>
+  <si>
+    <t>Ana Paula Paes</t>
+  </si>
+  <si>
+    <t>Sao Goncalo  / RJ</t>
+  </si>
+  <si>
+    <t>21 99114-5978</t>
+  </si>
+  <si>
+    <t>ENVIEI MENSAGEM / RESPONDEU que esta mudando para são gonçalo e gostaria de participar de um gc/ encaminhada para Niteroi</t>
+  </si>
+  <si>
+    <t>Luana Ramos</t>
+  </si>
+  <si>
+    <t>21 97445-9927</t>
+  </si>
+  <si>
+    <t>CRIS</t>
+  </si>
+  <si>
+    <t>Vanessa Spath</t>
+  </si>
+  <si>
+    <t>21 96706-1111</t>
+  </si>
+  <si>
+    <t>Gabriela Alves</t>
+  </si>
+  <si>
+    <t>21 98620-2503</t>
+  </si>
+  <si>
+    <t>CRIS - respondeu e pediu uma oração por se sentir muito cansada</t>
+  </si>
+  <si>
+    <t>Bruna Marques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santa Tereza </t>
+  </si>
+  <si>
+    <t>21 98198-3214</t>
+  </si>
+  <si>
+    <t>CRIS - conversando para encamiha-la a um gc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marie </t>
+  </si>
+  <si>
+    <t>21 97224-0352</t>
+  </si>
+  <si>
+    <t>CRIS - responde e estamos tentando encaminhar para um gc</t>
+  </si>
+  <si>
+    <t>Luana Somente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santo Cristo </t>
+  </si>
+  <si>
+    <t>21 98772-1266</t>
+  </si>
+  <si>
+    <t>DANI  - encaminhada para o gc. Supervisora Marcia</t>
+  </si>
+  <si>
+    <t>Izabela Oliveira</t>
+  </si>
+  <si>
+    <t>48 99934-6725</t>
+  </si>
+  <si>
+    <t>DANI  - trabalha embarcada 15 dias. Fará o start</t>
+  </si>
+  <si>
+    <t>Emilly Correia</t>
+  </si>
+  <si>
+    <t>Sampaio</t>
+  </si>
+  <si>
+    <t>21 97179-7808</t>
+  </si>
+  <si>
+    <t>DANI  - estava ocupada e vamos retornar para tentar encaminhar para um gc</t>
+  </si>
+  <si>
+    <t>Rubia Somente</t>
+  </si>
+  <si>
+    <t>21 98102-1716</t>
+  </si>
+  <si>
+    <t>DANI  - aceitou oração mas não quer ir ao start e nem gc</t>
+  </si>
+  <si>
+    <t>Juliana Monte</t>
+  </si>
+  <si>
+    <t>21 97034-7752</t>
+  </si>
+  <si>
+    <t>DANI  - encaminhada para gc de casais. Maryliz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lene </t>
+  </si>
+  <si>
+    <t>21 97719-6659</t>
+  </si>
+  <si>
+    <t>Bruna Lima</t>
+  </si>
+  <si>
+    <t>21 96717-3893</t>
+  </si>
+  <si>
+    <t>Natália Rodrigues Paiva</t>
+  </si>
+  <si>
+    <t>21 97161-5471</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marcela </t>
+  </si>
+  <si>
+    <t>21 98314-7362</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Larissa </t>
+  </si>
+  <si>
+    <t>21 97045-7685</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vandercleide </t>
+  </si>
+  <si>
+    <t>Nova Iguacu</t>
+  </si>
+  <si>
+    <t>21 98611-0767</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aline </t>
+  </si>
+  <si>
+    <t>Sao Conrado</t>
+  </si>
+  <si>
+    <t>21 21977-2093</t>
+  </si>
+  <si>
+    <t>Clara Xavier</t>
+  </si>
+  <si>
+    <t>21 21999-2825</t>
   </si>
 </sst>
 </file>
@@ -2385,10 +2736,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F662FB8-528C-4013-B4C5-67C7C16EE720}">
-  <dimension ref="A1:O181"/>
+  <dimension ref="A1:O219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
-      <selection activeCell="O166" sqref="O166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P180" sqref="P180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10914,6 +11265,1789 @@
         <v>24</v>
       </c>
     </row>
+    <row r="182" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A182" t="s">
+        <v>565</v>
+      </c>
+      <c r="B182" t="s">
+        <v>209</v>
+      </c>
+      <c r="C182" t="s">
+        <v>16</v>
+      </c>
+      <c r="D182" t="s">
+        <v>641</v>
+      </c>
+      <c r="E182" t="s">
+        <v>65</v>
+      </c>
+      <c r="F182" t="s">
+        <v>19</v>
+      </c>
+      <c r="G182">
+        <v>0</v>
+      </c>
+      <c r="H182" t="s">
+        <v>58</v>
+      </c>
+      <c r="I182" t="s">
+        <v>55</v>
+      </c>
+      <c r="J182" t="s">
+        <v>642</v>
+      </c>
+      <c r="K182" t="s">
+        <v>24</v>
+      </c>
+      <c r="L182" t="s">
+        <v>46</v>
+      </c>
+      <c r="M182" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N182" t="s">
+        <v>643</v>
+      </c>
+      <c r="O182" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A183" t="s">
+        <v>565</v>
+      </c>
+      <c r="B183" t="s">
+        <v>209</v>
+      </c>
+      <c r="C183" t="s">
+        <v>41</v>
+      </c>
+      <c r="D183" t="s">
+        <v>644</v>
+      </c>
+      <c r="E183" t="s">
+        <v>65</v>
+      </c>
+      <c r="F183" t="s">
+        <v>91</v>
+      </c>
+      <c r="G183">
+        <v>42</v>
+      </c>
+      <c r="H183" t="s">
+        <v>645</v>
+      </c>
+      <c r="I183" t="s">
+        <v>646</v>
+      </c>
+      <c r="J183" t="s">
+        <v>647</v>
+      </c>
+      <c r="K183" t="s">
+        <v>24</v>
+      </c>
+      <c r="L183" t="s">
+        <v>25</v>
+      </c>
+      <c r="M183" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N183" t="s">
+        <v>648</v>
+      </c>
+      <c r="O183" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="184" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A184" t="s">
+        <v>565</v>
+      </c>
+      <c r="B184" t="s">
+        <v>58</v>
+      </c>
+      <c r="C184" t="s">
+        <v>41</v>
+      </c>
+      <c r="D184" t="s">
+        <v>649</v>
+      </c>
+      <c r="E184" t="s">
+        <v>65</v>
+      </c>
+      <c r="F184" t="s">
+        <v>29</v>
+      </c>
+      <c r="G184">
+        <v>23</v>
+      </c>
+      <c r="H184" t="s">
+        <v>573</v>
+      </c>
+      <c r="I184" t="s">
+        <v>157</v>
+      </c>
+      <c r="J184" t="s">
+        <v>650</v>
+      </c>
+      <c r="K184" t="s">
+        <v>24</v>
+      </c>
+      <c r="L184" t="s">
+        <v>25</v>
+      </c>
+      <c r="M184" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N184" t="s">
+        <v>651</v>
+      </c>
+      <c r="O184" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="185" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A185" t="s">
+        <v>565</v>
+      </c>
+      <c r="B185" t="s">
+        <v>209</v>
+      </c>
+      <c r="C185" t="s">
+        <v>41</v>
+      </c>
+      <c r="D185" t="s">
+        <v>652</v>
+      </c>
+      <c r="E185" t="s">
+        <v>65</v>
+      </c>
+      <c r="F185" t="s">
+        <v>29</v>
+      </c>
+      <c r="G185">
+        <v>33</v>
+      </c>
+      <c r="H185" t="s">
+        <v>618</v>
+      </c>
+      <c r="I185" t="s">
+        <v>22</v>
+      </c>
+      <c r="J185" t="s">
+        <v>653</v>
+      </c>
+      <c r="K185" t="s">
+        <v>24</v>
+      </c>
+      <c r="L185" t="s">
+        <v>25</v>
+      </c>
+      <c r="M185" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N185" t="s">
+        <v>654</v>
+      </c>
+      <c r="O185" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="186" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A186" t="s">
+        <v>565</v>
+      </c>
+      <c r="B186" t="s">
+        <v>209</v>
+      </c>
+      <c r="C186" t="s">
+        <v>41</v>
+      </c>
+      <c r="D186" t="s">
+        <v>655</v>
+      </c>
+      <c r="E186" t="s">
+        <v>65</v>
+      </c>
+      <c r="F186" t="s">
+        <v>19</v>
+      </c>
+      <c r="G186">
+        <v>33</v>
+      </c>
+      <c r="H186" t="s">
+        <v>656</v>
+      </c>
+      <c r="I186" t="s">
+        <v>22</v>
+      </c>
+      <c r="J186" t="s">
+        <v>657</v>
+      </c>
+      <c r="K186" t="s">
+        <v>24</v>
+      </c>
+      <c r="L186" t="s">
+        <v>25</v>
+      </c>
+      <c r="M186" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N186" t="s">
+        <v>651</v>
+      </c>
+      <c r="O186" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="187" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A187" t="s">
+        <v>565</v>
+      </c>
+      <c r="B187" t="s">
+        <v>58</v>
+      </c>
+      <c r="C187" t="s">
+        <v>41</v>
+      </c>
+      <c r="D187" t="s">
+        <v>658</v>
+      </c>
+      <c r="E187" t="s">
+        <v>65</v>
+      </c>
+      <c r="F187" t="s">
+        <v>29</v>
+      </c>
+      <c r="G187">
+        <v>26</v>
+      </c>
+      <c r="H187" t="s">
+        <v>659</v>
+      </c>
+      <c r="I187" t="s">
+        <v>22</v>
+      </c>
+      <c r="J187" t="s">
+        <v>660</v>
+      </c>
+      <c r="K187" t="s">
+        <v>24</v>
+      </c>
+      <c r="L187" t="s">
+        <v>46</v>
+      </c>
+      <c r="M187" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N187" t="s">
+        <v>661</v>
+      </c>
+      <c r="O187" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="188" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A188" t="s">
+        <v>565</v>
+      </c>
+      <c r="B188" t="s">
+        <v>58</v>
+      </c>
+      <c r="C188" t="s">
+        <v>16</v>
+      </c>
+      <c r="D188" t="s">
+        <v>662</v>
+      </c>
+      <c r="E188" t="s">
+        <v>65</v>
+      </c>
+      <c r="F188" t="s">
+        <v>29</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
+      <c r="H188" t="s">
+        <v>58</v>
+      </c>
+      <c r="I188" t="s">
+        <v>55</v>
+      </c>
+      <c r="J188" t="s">
+        <v>663</v>
+      </c>
+      <c r="K188" t="s">
+        <v>24</v>
+      </c>
+      <c r="L188" t="s">
+        <v>201</v>
+      </c>
+      <c r="M188" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N188" t="s">
+        <v>661</v>
+      </c>
+      <c r="O188" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A189" t="s">
+        <v>565</v>
+      </c>
+      <c r="B189" t="s">
+        <v>209</v>
+      </c>
+      <c r="C189" t="s">
+        <v>41</v>
+      </c>
+      <c r="D189" t="s">
+        <v>664</v>
+      </c>
+      <c r="E189" t="s">
+        <v>65</v>
+      </c>
+      <c r="F189" t="s">
+        <v>29</v>
+      </c>
+      <c r="G189">
+        <v>35</v>
+      </c>
+      <c r="H189" t="s">
+        <v>665</v>
+      </c>
+      <c r="I189" t="s">
+        <v>22</v>
+      </c>
+      <c r="J189" t="s">
+        <v>666</v>
+      </c>
+      <c r="K189" t="s">
+        <v>24</v>
+      </c>
+      <c r="L189" t="s">
+        <v>25</v>
+      </c>
+      <c r="M189" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N189" t="s">
+        <v>661</v>
+      </c>
+      <c r="O189" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="190" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A190" t="s">
+        <v>565</v>
+      </c>
+      <c r="B190" t="s">
+        <v>209</v>
+      </c>
+      <c r="C190" t="s">
+        <v>27</v>
+      </c>
+      <c r="D190" t="s">
+        <v>667</v>
+      </c>
+      <c r="E190" t="s">
+        <v>65</v>
+      </c>
+      <c r="F190" t="s">
+        <v>29</v>
+      </c>
+      <c r="G190">
+        <v>25</v>
+      </c>
+      <c r="H190" t="s">
+        <v>281</v>
+      </c>
+      <c r="I190" t="s">
+        <v>22</v>
+      </c>
+      <c r="J190" t="s">
+        <v>668</v>
+      </c>
+      <c r="K190" t="s">
+        <v>24</v>
+      </c>
+      <c r="L190" t="s">
+        <v>25</v>
+      </c>
+      <c r="M190" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N190" t="s">
+        <v>661</v>
+      </c>
+      <c r="O190" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="191" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A191" t="s">
+        <v>565</v>
+      </c>
+      <c r="B191" t="s">
+        <v>209</v>
+      </c>
+      <c r="C191" t="s">
+        <v>41</v>
+      </c>
+      <c r="D191" t="s">
+        <v>669</v>
+      </c>
+      <c r="E191" t="s">
+        <v>65</v>
+      </c>
+      <c r="F191" t="s">
+        <v>29</v>
+      </c>
+      <c r="G191">
+        <v>30</v>
+      </c>
+      <c r="H191" t="s">
+        <v>44</v>
+      </c>
+      <c r="I191" t="s">
+        <v>22</v>
+      </c>
+      <c r="J191" t="s">
+        <v>670</v>
+      </c>
+      <c r="K191" t="s">
+        <v>24</v>
+      </c>
+      <c r="L191" t="s">
+        <v>46</v>
+      </c>
+      <c r="M191" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N191" t="s">
+        <v>661</v>
+      </c>
+      <c r="O191" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A192" t="s">
+        <v>565</v>
+      </c>
+      <c r="B192" t="s">
+        <v>58</v>
+      </c>
+      <c r="C192" t="s">
+        <v>41</v>
+      </c>
+      <c r="D192" t="s">
+        <v>671</v>
+      </c>
+      <c r="E192" t="s">
+        <v>65</v>
+      </c>
+      <c r="F192" t="s">
+        <v>91</v>
+      </c>
+      <c r="G192">
+        <v>71</v>
+      </c>
+      <c r="H192" t="s">
+        <v>296</v>
+      </c>
+      <c r="I192" t="s">
+        <v>22</v>
+      </c>
+      <c r="J192" t="s">
+        <v>672</v>
+      </c>
+      <c r="K192" t="s">
+        <v>24</v>
+      </c>
+      <c r="L192" t="s">
+        <v>25</v>
+      </c>
+      <c r="M192" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N192" t="s">
+        <v>673</v>
+      </c>
+      <c r="O192" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A193" t="s">
+        <v>565</v>
+      </c>
+      <c r="B193" t="s">
+        <v>209</v>
+      </c>
+      <c r="C193" t="s">
+        <v>27</v>
+      </c>
+      <c r="D193" t="s">
+        <v>674</v>
+      </c>
+      <c r="E193" t="s">
+        <v>65</v>
+      </c>
+      <c r="F193" t="s">
+        <v>19</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
+      <c r="H193" t="s">
+        <v>573</v>
+      </c>
+      <c r="I193" t="s">
+        <v>675</v>
+      </c>
+      <c r="J193" t="s">
+        <v>676</v>
+      </c>
+      <c r="K193" t="s">
+        <v>24</v>
+      </c>
+      <c r="L193" t="s">
+        <v>46</v>
+      </c>
+      <c r="M193" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N193" t="s">
+        <v>677</v>
+      </c>
+      <c r="O193" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A194" t="s">
+        <v>565</v>
+      </c>
+      <c r="B194" t="s">
+        <v>209</v>
+      </c>
+      <c r="C194" t="s">
+        <v>16</v>
+      </c>
+      <c r="D194" t="s">
+        <v>678</v>
+      </c>
+      <c r="E194" t="s">
+        <v>65</v>
+      </c>
+      <c r="F194" t="s">
+        <v>19</v>
+      </c>
+      <c r="G194">
+        <v>49</v>
+      </c>
+      <c r="H194" t="s">
+        <v>679</v>
+      </c>
+      <c r="I194" t="s">
+        <v>157</v>
+      </c>
+      <c r="J194" t="s">
+        <v>680</v>
+      </c>
+      <c r="K194" t="s">
+        <v>24</v>
+      </c>
+      <c r="L194" t="s">
+        <v>457</v>
+      </c>
+      <c r="M194" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N194" t="s">
+        <v>681</v>
+      </c>
+      <c r="O194" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A195" t="s">
+        <v>565</v>
+      </c>
+      <c r="B195" t="s">
+        <v>209</v>
+      </c>
+      <c r="C195" t="s">
+        <v>27</v>
+      </c>
+      <c r="D195" t="s">
+        <v>682</v>
+      </c>
+      <c r="E195" t="s">
+        <v>65</v>
+      </c>
+      <c r="F195" t="s">
+        <v>91</v>
+      </c>
+      <c r="G195">
+        <v>0</v>
+      </c>
+      <c r="H195" t="s">
+        <v>58</v>
+      </c>
+      <c r="I195" t="s">
+        <v>683</v>
+      </c>
+      <c r="J195" t="s">
+        <v>684</v>
+      </c>
+      <c r="K195" t="s">
+        <v>24</v>
+      </c>
+      <c r="L195" t="s">
+        <v>46</v>
+      </c>
+      <c r="M195" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N195" t="s">
+        <v>685</v>
+      </c>
+      <c r="O195" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A196" t="s">
+        <v>565</v>
+      </c>
+      <c r="B196" t="s">
+        <v>58</v>
+      </c>
+      <c r="C196" t="s">
+        <v>16</v>
+      </c>
+      <c r="D196" t="s">
+        <v>686</v>
+      </c>
+      <c r="E196" t="s">
+        <v>65</v>
+      </c>
+      <c r="F196" t="s">
+        <v>29</v>
+      </c>
+      <c r="G196">
+        <v>18</v>
+      </c>
+      <c r="H196" t="s">
+        <v>231</v>
+      </c>
+      <c r="I196" t="s">
+        <v>335</v>
+      </c>
+      <c r="J196" t="s">
+        <v>687</v>
+      </c>
+      <c r="K196" t="s">
+        <v>24</v>
+      </c>
+      <c r="L196" t="s">
+        <v>25</v>
+      </c>
+      <c r="M196" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N196" t="s">
+        <v>688</v>
+      </c>
+      <c r="O196" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>565</v>
+      </c>
+      <c r="B197" t="s">
+        <v>209</v>
+      </c>
+      <c r="C197" t="s">
+        <v>41</v>
+      </c>
+      <c r="D197" t="s">
+        <v>689</v>
+      </c>
+      <c r="E197" t="s">
+        <v>65</v>
+      </c>
+      <c r="F197" t="s">
+        <v>29</v>
+      </c>
+      <c r="G197">
+        <v>25</v>
+      </c>
+      <c r="H197" t="s">
+        <v>690</v>
+      </c>
+      <c r="I197" t="s">
+        <v>691</v>
+      </c>
+      <c r="J197" t="s">
+        <v>692</v>
+      </c>
+      <c r="K197" t="s">
+        <v>24</v>
+      </c>
+      <c r="L197" t="s">
+        <v>46</v>
+      </c>
+      <c r="M197" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N197" t="s">
+        <v>693</v>
+      </c>
+      <c r="O197" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>565</v>
+      </c>
+      <c r="B198" t="s">
+        <v>58</v>
+      </c>
+      <c r="C198" t="s">
+        <v>27</v>
+      </c>
+      <c r="D198" t="s">
+        <v>694</v>
+      </c>
+      <c r="E198" t="s">
+        <v>65</v>
+      </c>
+      <c r="F198" t="s">
+        <v>29</v>
+      </c>
+      <c r="G198">
+        <v>33</v>
+      </c>
+      <c r="H198" t="s">
+        <v>58</v>
+      </c>
+      <c r="I198" t="s">
+        <v>55</v>
+      </c>
+      <c r="J198" t="s">
+        <v>695</v>
+      </c>
+      <c r="K198" t="s">
+        <v>24</v>
+      </c>
+      <c r="L198" t="s">
+        <v>25</v>
+      </c>
+      <c r="M198" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N198" t="s">
+        <v>693</v>
+      </c>
+      <c r="O198" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>565</v>
+      </c>
+      <c r="B199" t="s">
+        <v>58</v>
+      </c>
+      <c r="C199" t="s">
+        <v>27</v>
+      </c>
+      <c r="D199" t="s">
+        <v>696</v>
+      </c>
+      <c r="E199" t="s">
+        <v>65</v>
+      </c>
+      <c r="F199" t="s">
+        <v>19</v>
+      </c>
+      <c r="G199">
+        <v>47</v>
+      </c>
+      <c r="H199" t="s">
+        <v>166</v>
+      </c>
+      <c r="I199" t="s">
+        <v>22</v>
+      </c>
+      <c r="J199" t="s">
+        <v>697</v>
+      </c>
+      <c r="K199" t="s">
+        <v>24</v>
+      </c>
+      <c r="L199" t="s">
+        <v>25</v>
+      </c>
+      <c r="M199" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N199" t="s">
+        <v>698</v>
+      </c>
+      <c r="O199" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>565</v>
+      </c>
+      <c r="B200" t="s">
+        <v>58</v>
+      </c>
+      <c r="C200" t="s">
+        <v>16</v>
+      </c>
+      <c r="D200" t="s">
+        <v>699</v>
+      </c>
+      <c r="E200" t="s">
+        <v>65</v>
+      </c>
+      <c r="F200" t="s">
+        <v>91</v>
+      </c>
+      <c r="G200">
+        <v>41</v>
+      </c>
+      <c r="H200" t="s">
+        <v>700</v>
+      </c>
+      <c r="I200" t="s">
+        <v>701</v>
+      </c>
+      <c r="J200" t="s">
+        <v>702</v>
+      </c>
+      <c r="K200" t="s">
+        <v>24</v>
+      </c>
+      <c r="L200" t="s">
+        <v>25</v>
+      </c>
+      <c r="M200" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N200" t="s">
+        <v>703</v>
+      </c>
+      <c r="O200" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>565</v>
+      </c>
+      <c r="B201" t="s">
+        <v>58</v>
+      </c>
+      <c r="C201" t="s">
+        <v>41</v>
+      </c>
+      <c r="D201" t="s">
+        <v>704</v>
+      </c>
+      <c r="E201" t="s">
+        <v>65</v>
+      </c>
+      <c r="F201" t="s">
+        <v>29</v>
+      </c>
+      <c r="G201">
+        <v>35</v>
+      </c>
+      <c r="I201" t="s">
+        <v>705</v>
+      </c>
+      <c r="J201" t="s">
+        <v>706</v>
+      </c>
+      <c r="K201" t="s">
+        <v>24</v>
+      </c>
+      <c r="L201" t="s">
+        <v>148</v>
+      </c>
+      <c r="M201" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N201" t="s">
+        <v>707</v>
+      </c>
+      <c r="O201" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>565</v>
+      </c>
+      <c r="B202" t="s">
+        <v>58</v>
+      </c>
+      <c r="C202" t="s">
+        <v>16</v>
+      </c>
+      <c r="D202" t="s">
+        <v>708</v>
+      </c>
+      <c r="E202" t="s">
+        <v>65</v>
+      </c>
+      <c r="F202" t="s">
+        <v>58</v>
+      </c>
+      <c r="G202">
+        <v>34</v>
+      </c>
+      <c r="H202" t="s">
+        <v>58</v>
+      </c>
+      <c r="I202" t="s">
+        <v>55</v>
+      </c>
+      <c r="J202" t="s">
+        <v>709</v>
+      </c>
+      <c r="K202" t="s">
+        <v>24</v>
+      </c>
+      <c r="L202" t="s">
+        <v>25</v>
+      </c>
+      <c r="M202" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N202" t="s">
+        <v>710</v>
+      </c>
+      <c r="O202" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A203" t="s">
+        <v>565</v>
+      </c>
+      <c r="B203" t="s">
+        <v>209</v>
+      </c>
+      <c r="C203" t="s">
+        <v>27</v>
+      </c>
+      <c r="D203" t="s">
+        <v>711</v>
+      </c>
+      <c r="E203" t="s">
+        <v>65</v>
+      </c>
+      <c r="F203" t="s">
+        <v>91</v>
+      </c>
+      <c r="G203">
+        <v>41</v>
+      </c>
+      <c r="H203" t="s">
+        <v>166</v>
+      </c>
+      <c r="I203" t="s">
+        <v>22</v>
+      </c>
+      <c r="J203" t="s">
+        <v>712</v>
+      </c>
+      <c r="K203" t="s">
+        <v>24</v>
+      </c>
+      <c r="L203" t="s">
+        <v>25</v>
+      </c>
+      <c r="M203" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N203" t="s">
+        <v>710</v>
+      </c>
+      <c r="O203" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>565</v>
+      </c>
+      <c r="B204" t="s">
+        <v>209</v>
+      </c>
+      <c r="C204" t="s">
+        <v>27</v>
+      </c>
+      <c r="D204" t="s">
+        <v>713</v>
+      </c>
+      <c r="E204" t="s">
+        <v>65</v>
+      </c>
+      <c r="F204" t="s">
+        <v>29</v>
+      </c>
+      <c r="G204">
+        <v>31</v>
+      </c>
+      <c r="H204" t="s">
+        <v>58</v>
+      </c>
+      <c r="I204" t="s">
+        <v>55</v>
+      </c>
+      <c r="J204" t="s">
+        <v>714</v>
+      </c>
+      <c r="K204" t="s">
+        <v>24</v>
+      </c>
+      <c r="L204" t="s">
+        <v>25</v>
+      </c>
+      <c r="M204" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N204" t="s">
+        <v>715</v>
+      </c>
+      <c r="O204" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>565</v>
+      </c>
+      <c r="B205" t="s">
+        <v>209</v>
+      </c>
+      <c r="C205" t="s">
+        <v>41</v>
+      </c>
+      <c r="D205" t="s">
+        <v>716</v>
+      </c>
+      <c r="E205" t="s">
+        <v>65</v>
+      </c>
+      <c r="F205" t="s">
+        <v>29</v>
+      </c>
+      <c r="G205">
+        <v>41</v>
+      </c>
+      <c r="H205" t="s">
+        <v>717</v>
+      </c>
+      <c r="I205" t="s">
+        <v>157</v>
+      </c>
+      <c r="J205" t="s">
+        <v>718</v>
+      </c>
+      <c r="K205" t="s">
+        <v>24</v>
+      </c>
+      <c r="L205" t="s">
+        <v>25</v>
+      </c>
+      <c r="M205" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N205" t="s">
+        <v>719</v>
+      </c>
+      <c r="O205" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>565</v>
+      </c>
+      <c r="B206" t="s">
+        <v>209</v>
+      </c>
+      <c r="C206" t="s">
+        <v>16</v>
+      </c>
+      <c r="D206" t="s">
+        <v>720</v>
+      </c>
+      <c r="E206" t="s">
+        <v>65</v>
+      </c>
+      <c r="F206" t="s">
+        <v>29</v>
+      </c>
+      <c r="G206">
+        <v>43</v>
+      </c>
+      <c r="H206" t="s">
+        <v>58</v>
+      </c>
+      <c r="I206" t="s">
+        <v>55</v>
+      </c>
+      <c r="J206" t="s">
+        <v>721</v>
+      </c>
+      <c r="K206" t="s">
+        <v>24</v>
+      </c>
+      <c r="L206" t="s">
+        <v>445</v>
+      </c>
+      <c r="M206" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N206" t="s">
+        <v>722</v>
+      </c>
+      <c r="O206" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>589</v>
+      </c>
+      <c r="B207" t="s">
+        <v>209</v>
+      </c>
+      <c r="C207" t="s">
+        <v>27</v>
+      </c>
+      <c r="D207" t="s">
+        <v>723</v>
+      </c>
+      <c r="E207" t="s">
+        <v>65</v>
+      </c>
+      <c r="F207" t="s">
+        <v>58</v>
+      </c>
+      <c r="G207">
+        <v>100</v>
+      </c>
+      <c r="H207" t="s">
+        <v>724</v>
+      </c>
+      <c r="I207" t="s">
+        <v>55</v>
+      </c>
+      <c r="J207" t="s">
+        <v>725</v>
+      </c>
+      <c r="K207" t="s">
+        <v>24</v>
+      </c>
+      <c r="L207" t="s">
+        <v>25</v>
+      </c>
+      <c r="M207" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N207" t="s">
+        <v>726</v>
+      </c>
+      <c r="O207" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>589</v>
+      </c>
+      <c r="B208" t="s">
+        <v>58</v>
+      </c>
+      <c r="C208" t="s">
+        <v>27</v>
+      </c>
+      <c r="D208" t="s">
+        <v>727</v>
+      </c>
+      <c r="E208" t="s">
+        <v>65</v>
+      </c>
+      <c r="F208" t="s">
+        <v>29</v>
+      </c>
+      <c r="G208">
+        <v>29</v>
+      </c>
+      <c r="H208" t="s">
+        <v>516</v>
+      </c>
+      <c r="I208" t="s">
+        <v>55</v>
+      </c>
+      <c r="J208" t="s">
+        <v>728</v>
+      </c>
+      <c r="K208" t="s">
+        <v>24</v>
+      </c>
+      <c r="L208" t="s">
+        <v>25</v>
+      </c>
+      <c r="M208" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N208" t="s">
+        <v>729</v>
+      </c>
+      <c r="O208" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A209" t="s">
+        <v>589</v>
+      </c>
+      <c r="B209" t="s">
+        <v>209</v>
+      </c>
+      <c r="C209" t="s">
+        <v>41</v>
+      </c>
+      <c r="D209" t="s">
+        <v>730</v>
+      </c>
+      <c r="E209" t="s">
+        <v>65</v>
+      </c>
+      <c r="F209" t="s">
+        <v>29</v>
+      </c>
+      <c r="G209">
+        <v>25</v>
+      </c>
+      <c r="H209" t="s">
+        <v>731</v>
+      </c>
+      <c r="I209" t="s">
+        <v>22</v>
+      </c>
+      <c r="J209" t="s">
+        <v>732</v>
+      </c>
+      <c r="K209" t="s">
+        <v>24</v>
+      </c>
+      <c r="L209" t="s">
+        <v>25</v>
+      </c>
+      <c r="M209" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N209" t="s">
+        <v>733</v>
+      </c>
+      <c r="O209" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="210" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>589</v>
+      </c>
+      <c r="B210" t="s">
+        <v>209</v>
+      </c>
+      <c r="C210" t="s">
+        <v>27</v>
+      </c>
+      <c r="D210" t="s">
+        <v>734</v>
+      </c>
+      <c r="E210" t="s">
+        <v>65</v>
+      </c>
+      <c r="F210" t="s">
+        <v>58</v>
+      </c>
+      <c r="G210">
+        <v>0</v>
+      </c>
+      <c r="H210" t="s">
+        <v>58</v>
+      </c>
+      <c r="I210" t="s">
+        <v>55</v>
+      </c>
+      <c r="J210" t="s">
+        <v>735</v>
+      </c>
+      <c r="K210" t="s">
+        <v>24</v>
+      </c>
+      <c r="L210" t="s">
+        <v>25</v>
+      </c>
+      <c r="M210" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N210" t="s">
+        <v>736</v>
+      </c>
+      <c r="O210" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="211" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>589</v>
+      </c>
+      <c r="B211" t="s">
+        <v>209</v>
+      </c>
+      <c r="C211" t="s">
+        <v>41</v>
+      </c>
+      <c r="D211" t="s">
+        <v>737</v>
+      </c>
+      <c r="E211" t="s">
+        <v>65</v>
+      </c>
+      <c r="F211" t="s">
+        <v>19</v>
+      </c>
+      <c r="G211">
+        <v>24</v>
+      </c>
+      <c r="H211" t="s">
+        <v>152</v>
+      </c>
+      <c r="I211" t="s">
+        <v>420</v>
+      </c>
+      <c r="J211" t="s">
+        <v>738</v>
+      </c>
+      <c r="K211" t="s">
+        <v>24</v>
+      </c>
+      <c r="L211" t="s">
+        <v>25</v>
+      </c>
+      <c r="M211" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N211" t="s">
+        <v>739</v>
+      </c>
+      <c r="O211" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="212" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>589</v>
+      </c>
+      <c r="B212" t="s">
+        <v>209</v>
+      </c>
+      <c r="C212" t="s">
+        <v>16</v>
+      </c>
+      <c r="D212" t="s">
+        <v>740</v>
+      </c>
+      <c r="E212" t="s">
+        <v>65</v>
+      </c>
+      <c r="F212" t="s">
+        <v>29</v>
+      </c>
+      <c r="G212">
+        <v>35</v>
+      </c>
+      <c r="H212" t="s">
+        <v>58</v>
+      </c>
+      <c r="I212" t="s">
+        <v>55</v>
+      </c>
+      <c r="J212" t="s">
+        <v>741</v>
+      </c>
+      <c r="K212" t="s">
+        <v>24</v>
+      </c>
+      <c r="L212" t="s">
+        <v>25</v>
+      </c>
+      <c r="M212" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N212" t="s">
+        <v>58</v>
+      </c>
+      <c r="O212" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="213" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>589</v>
+      </c>
+      <c r="B213" t="s">
+        <v>209</v>
+      </c>
+      <c r="C213" t="s">
+        <v>27</v>
+      </c>
+      <c r="D213" t="s">
+        <v>742</v>
+      </c>
+      <c r="E213" t="s">
+        <v>65</v>
+      </c>
+      <c r="F213" t="s">
+        <v>29</v>
+      </c>
+      <c r="G213">
+        <v>29</v>
+      </c>
+      <c r="H213" t="s">
+        <v>618</v>
+      </c>
+      <c r="I213" t="s">
+        <v>22</v>
+      </c>
+      <c r="J213" t="s">
+        <v>743</v>
+      </c>
+      <c r="K213" t="s">
+        <v>24</v>
+      </c>
+      <c r="L213" t="s">
+        <v>25</v>
+      </c>
+      <c r="M213" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N213" t="s">
+        <v>58</v>
+      </c>
+      <c r="O213" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="214" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>589</v>
+      </c>
+      <c r="B214" t="s">
+        <v>209</v>
+      </c>
+      <c r="C214" t="s">
+        <v>41</v>
+      </c>
+      <c r="D214" t="s">
+        <v>744</v>
+      </c>
+      <c r="E214" t="s">
+        <v>65</v>
+      </c>
+      <c r="F214" t="s">
+        <v>19</v>
+      </c>
+      <c r="G214">
+        <v>22</v>
+      </c>
+      <c r="H214" t="s">
+        <v>129</v>
+      </c>
+      <c r="I214" t="s">
+        <v>22</v>
+      </c>
+      <c r="J214" t="s">
+        <v>745</v>
+      </c>
+      <c r="K214" t="s">
+        <v>24</v>
+      </c>
+      <c r="L214" t="s">
+        <v>46</v>
+      </c>
+      <c r="M214" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N214" t="s">
+        <v>58</v>
+      </c>
+      <c r="O214" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="215" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>589</v>
+      </c>
+      <c r="B215" t="s">
+        <v>209</v>
+      </c>
+      <c r="C215" t="s">
+        <v>27</v>
+      </c>
+      <c r="D215" t="s">
+        <v>746</v>
+      </c>
+      <c r="E215" t="s">
+        <v>65</v>
+      </c>
+      <c r="F215" t="s">
+        <v>58</v>
+      </c>
+      <c r="G215">
+        <v>0</v>
+      </c>
+      <c r="H215" t="s">
+        <v>129</v>
+      </c>
+      <c r="I215" t="s">
+        <v>55</v>
+      </c>
+      <c r="J215" t="s">
+        <v>747</v>
+      </c>
+      <c r="K215" t="s">
+        <v>24</v>
+      </c>
+      <c r="L215" t="s">
+        <v>25</v>
+      </c>
+      <c r="M215" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N215" t="s">
+        <v>58</v>
+      </c>
+      <c r="O215" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="216" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>589</v>
+      </c>
+      <c r="B216" t="s">
+        <v>209</v>
+      </c>
+      <c r="C216" t="s">
+        <v>27</v>
+      </c>
+      <c r="D216" t="s">
+        <v>748</v>
+      </c>
+      <c r="E216" t="s">
+        <v>65</v>
+      </c>
+      <c r="F216" t="s">
+        <v>58</v>
+      </c>
+      <c r="G216">
+        <v>0</v>
+      </c>
+      <c r="H216" t="s">
+        <v>281</v>
+      </c>
+      <c r="I216" t="s">
+        <v>85</v>
+      </c>
+      <c r="J216" t="s">
+        <v>749</v>
+      </c>
+      <c r="K216" t="s">
+        <v>24</v>
+      </c>
+      <c r="L216" t="s">
+        <v>25</v>
+      </c>
+      <c r="M216" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N216" t="s">
+        <v>58</v>
+      </c>
+      <c r="O216" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>589</v>
+      </c>
+      <c r="B217" t="s">
+        <v>209</v>
+      </c>
+      <c r="C217" t="s">
+        <v>27</v>
+      </c>
+      <c r="D217" t="s">
+        <v>750</v>
+      </c>
+      <c r="E217" t="s">
+        <v>65</v>
+      </c>
+      <c r="F217" t="s">
+        <v>58</v>
+      </c>
+      <c r="G217">
+        <v>0</v>
+      </c>
+      <c r="H217" t="s">
+        <v>751</v>
+      </c>
+      <c r="I217" t="s">
+        <v>36</v>
+      </c>
+      <c r="J217" t="s">
+        <v>752</v>
+      </c>
+      <c r="K217" t="s">
+        <v>24</v>
+      </c>
+      <c r="L217" t="s">
+        <v>25</v>
+      </c>
+      <c r="M217" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N217" t="s">
+        <v>58</v>
+      </c>
+      <c r="O217" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="218" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>589</v>
+      </c>
+      <c r="B218" t="s">
+        <v>209</v>
+      </c>
+      <c r="C218" t="s">
+        <v>27</v>
+      </c>
+      <c r="D218" t="s">
+        <v>753</v>
+      </c>
+      <c r="E218" t="s">
+        <v>65</v>
+      </c>
+      <c r="F218" t="s">
+        <v>58</v>
+      </c>
+      <c r="G218">
+        <v>0</v>
+      </c>
+      <c r="H218" t="s">
+        <v>754</v>
+      </c>
+      <c r="I218" t="s">
+        <v>36</v>
+      </c>
+      <c r="J218" t="s">
+        <v>755</v>
+      </c>
+      <c r="K218" t="s">
+        <v>24</v>
+      </c>
+      <c r="L218" t="s">
+        <v>25</v>
+      </c>
+      <c r="M218" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N218" t="s">
+        <v>58</v>
+      </c>
+      <c r="O218" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="219" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>589</v>
+      </c>
+      <c r="B219" t="s">
+        <v>209</v>
+      </c>
+      <c r="C219" t="s">
+        <v>27</v>
+      </c>
+      <c r="D219" t="s">
+        <v>756</v>
+      </c>
+      <c r="E219" t="s">
+        <v>65</v>
+      </c>
+      <c r="F219" t="s">
+        <v>58</v>
+      </c>
+      <c r="G219">
+        <v>0</v>
+      </c>
+      <c r="H219" t="s">
+        <v>178</v>
+      </c>
+      <c r="I219" t="s">
+        <v>36</v>
+      </c>
+      <c r="J219" t="s">
+        <v>757</v>
+      </c>
+      <c r="K219" t="s">
+        <v>24</v>
+      </c>
+      <c r="L219" t="s">
+        <v>25</v>
+      </c>
+      <c r="M219" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N219" t="s">
+        <v>58</v>
+      </c>
+      <c r="O219" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O157">
     <sortCondition descending="1" ref="A6:A157"/>

</xml_diff>